<commit_message>
reporte: por sector ok
</commit_message>
<xml_diff>
--- a/public/Reporte por Sector.xlsx
+++ b/public/Reporte por Sector.xlsx
@@ -20,13 +20,13 @@
     <t>FORMATO - RESUMEN DE TRABAJO DIARIO EN VIGILANCIA Y CONTROL DEL AEDES AEGYPTI</t>
   </si>
   <si>
-    <t>Responsable</t>
-  </si>
-  <si>
-    <t>Localidad</t>
-  </si>
-  <si>
-    <t>VICE</t>
+    <t>Responsable:</t>
+  </si>
+  <si>
+    <t>Localidad:</t>
+  </si>
+  <si>
+    <t>E.S:</t>
   </si>
   <si>
     <t>N°</t>
@@ -65,13 +65,13 @@
     <t>Tratadas</t>
   </si>
   <si>
-    <t>Tanque alto</t>
+    <t>Tanque elevado</t>
   </si>
   <si>
     <t>Tanque bajo</t>
   </si>
   <si>
-    <t>Cilindro</t>
+    <t>Cilindros</t>
   </si>
   <si>
     <t>Sansón</t>
@@ -113,7 +113,7 @@
     <t>Total Gasto IGR</t>
   </si>
   <si>
-    <t>gr</t>
+    <t>(gr)</t>
   </si>
   <si>
     <t>SECTOR 123</t>
@@ -536,10 +536,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AW43"/>
+  <dimension ref="A1:AT43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A11" sqref="A11:AW11"/>
+      <selection activeCell="A11" sqref="A11:AT11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -586,25 +586,22 @@
     <col min="40" max="40" width="4" customWidth="true" style="0"/>
     <col min="41" max="41" width="4" customWidth="true" style="0"/>
     <col min="42" max="42" width="4" customWidth="true" style="0"/>
-    <col min="43" max="43" width="4" customWidth="true" style="0"/>
-    <col min="44" max="44" width="4" customWidth="true" style="0"/>
-    <col min="45" max="45" width="4" customWidth="true" style="0"/>
+    <col min="43" max="43" width="6" customWidth="true" style="0"/>
+    <col min="44" max="44" width="6" customWidth="true" style="0"/>
+    <col min="45" max="45" width="6" customWidth="true" style="0"/>
     <col min="46" max="46" width="6" customWidth="true" style="0"/>
-    <col min="47" max="47" width="6" customWidth="true" style="0"/>
-    <col min="48" max="48" width="6" customWidth="true" style="0"/>
-    <col min="49" max="49" width="6" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49">
+    <row r="1" spans="1:46">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:49" customHeight="1" ht="25">
+    <row r="2" spans="1:46" customHeight="1" ht="25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:49"/>
-    <row r="4" spans="1:49">
+    <row r="3" spans="1:46"/>
+    <row r="4" spans="1:46">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -622,18 +619,24 @@
       <c r="O4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="U4" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="U4" s="3"/>
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
       <c r="Y4" s="3"/>
       <c r="Z4" s="3"/>
       <c r="AA4" s="3"/>
-    </row>
-    <row r="5" spans="1:49"/>
-    <row r="6" spans="1:49">
+      <c r="AC4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
+      <c r="AG4" s="3"/>
+      <c r="AH4" s="3"/>
+      <c r="AI4" s="3"/>
+    </row>
+    <row r="5" spans="1:46"/>
+    <row r="6" spans="1:46">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -684,19 +687,16 @@
       <c r="AN6" s="5"/>
       <c r="AO6" s="5"/>
       <c r="AP6" s="5"/>
-      <c r="AQ6" s="5"/>
+      <c r="AQ6" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="AR6" s="5"/>
       <c r="AS6" s="5"/>
       <c r="AT6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AU6" s="5"/>
-      <c r="AV6" s="5"/>
-      <c r="AW6" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:49" customHeight="1" ht="40">
+    <row r="7" spans="1:46" customHeight="1" ht="40">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6" t="s">
@@ -761,31 +761,26 @@
       <c r="AF7" s="5"/>
       <c r="AG7" s="5"/>
       <c r="AH7" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AI7" s="5"/>
       <c r="AJ7" s="5"/>
       <c r="AK7" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AL7" s="5"/>
       <c r="AM7" s="5"/>
       <c r="AN7" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AO7" s="5"/>
       <c r="AP7" s="5"/>
-      <c r="AQ7" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="AQ7" s="6"/>
       <c r="AR7" s="5"/>
       <c r="AS7" s="5"/>
       <c r="AT7" s="6"/>
-      <c r="AU7" s="5"/>
-      <c r="AV7" s="5"/>
-      <c r="AW7" s="6"/>
-    </row>
-    <row r="8" spans="1:49">
+    </row>
+    <row r="8" spans="1:46">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -832,11 +827,8 @@
       <c r="AR8" s="5"/>
       <c r="AS8" s="5"/>
       <c r="AT8" s="5"/>
-      <c r="AU8" s="5"/>
-      <c r="AV8" s="5"/>
-      <c r="AW8" s="5"/>
-    </row>
-    <row r="9" spans="1:49">
+    </row>
+    <row r="9" spans="1:46">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -949,36 +941,25 @@
         <v>27</v>
       </c>
       <c r="AR9" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="AS9" s="5" t="s">
         <v>29</v>
       </c>
       <c r="AT9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="AU9" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="AV9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="AW9" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:49">
+    <row r="10" spans="1:46">
       <c r="A10" s="7">
         <v>1</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="7"/>
+      <c r="D10" s="7">
         <v>0</v>
-      </c>
-      <c r="D10" s="7">
-        <v>2</v>
       </c>
       <c r="E10" s="7">
         <v>0</v>
@@ -987,148 +968,77 @@
         <v>0</v>
       </c>
       <c r="G10" s="7">
+        <v>2</v>
+      </c>
+      <c r="H10" s="7">
+        <f>SUM(K10,N10,Q10,T10,W10,Z10,AC10,AF10,AI10,AL10,AO10)</f>
         <v>0</v>
       </c>
-      <c r="H10" s="7">
+      <c r="I10" s="7">
+        <f>SUM(L10,O10,R10,U10,X10,AA10,AD10,AG10,AJ10,AM10,AP10)</f>
         <v>0</v>
       </c>
-      <c r="I10" s="7">
+      <c r="J10" s="7">
+        <v>15</v>
+      </c>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7">
+        <v>9</v>
+      </c>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
+      <c r="AG10" s="7"/>
+      <c r="AH10" s="7"/>
+      <c r="AI10" s="7"/>
+      <c r="AJ10" s="7"/>
+      <c r="AK10" s="7"/>
+      <c r="AL10" s="7"/>
+      <c r="AM10" s="7"/>
+      <c r="AN10" s="7"/>
+      <c r="AO10" s="7"/>
+      <c r="AP10" s="7"/>
+      <c r="AQ10" s="7">
+        <f>SUM(J10,M10,P10,S10,V10,Y10,AB10,AE10,AH10,AK10,AN10)</f>
+        <v>24</v>
+      </c>
+      <c r="AR10" s="7">
+        <f>SUM(K10,N10,Q10,T10,W10,Z10,AC10,AF10,AI10,AL10,AO10)</f>
         <v>0</v>
       </c>
-      <c r="J10" s="7">
-        <v>1</v>
-      </c>
-      <c r="K10" s="7">
+      <c r="AS10" s="7">
+        <f>SUM(L10,O10,R10,U10,X10,AA10,AD10,AG10,AJ10,AM10,AP10)</f>
         <v>0</v>
       </c>
-      <c r="L10" s="7">
-        <v>0</v>
-      </c>
-      <c r="M10" s="7">
-        <v>0</v>
-      </c>
-      <c r="N10" s="7">
-        <v>0</v>
-      </c>
-      <c r="O10" s="7">
-        <v>0</v>
-      </c>
-      <c r="P10" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="7">
-        <v>0</v>
-      </c>
-      <c r="R10" s="7">
-        <v>0</v>
-      </c>
-      <c r="S10" s="7">
-        <v>0</v>
-      </c>
-      <c r="T10" s="7">
-        <v>0</v>
-      </c>
-      <c r="U10" s="7">
-        <v>0</v>
-      </c>
-      <c r="V10" s="7">
-        <v>0</v>
-      </c>
-      <c r="W10" s="7">
-        <v>0</v>
-      </c>
-      <c r="X10" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AE10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AH10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AI10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AJ10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AK10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AL10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AM10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AN10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AO10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AP10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AQ10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AR10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AS10" s="7">
-        <v>0</v>
-      </c>
-      <c r="AT10" s="7">
-        <f>SUM(J10:AS10)</f>
-        <v>1</v>
-      </c>
-      <c r="AU10" s="7">
-        <f>SUM(J10:AS10)</f>
-        <v>1</v>
-      </c>
-      <c r="AV10" s="7">
-        <f>SUM(J10:AS10)</f>
-        <v>1</v>
-      </c>
-      <c r="AW10" s="7"/>
-    </row>
-    <row r="11" spans="1:49">
+      <c r="AT10" s="7"/>
+    </row>
+    <row r="11" spans="1:46">
       <c r="A11" s="7">
         <v>2</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="7"/>
+      <c r="D11" s="7">
         <v>0</v>
-      </c>
-      <c r="D11" s="7">
-        <v>1</v>
       </c>
       <c r="E11" s="7">
         <v>0</v>
@@ -1137,137 +1047,70 @@
         <v>0</v>
       </c>
       <c r="G11" s="7">
+        <v>1</v>
+      </c>
+      <c r="H11" s="7">
+        <f>SUM(K11,N11,Q11,T11,W11,Z11,AC11,AF11,AI11,AL11,AO11)</f>
+        <v>3</v>
+      </c>
+      <c r="I11" s="7">
+        <f>SUM(L11,O11,R11,U11,X11,AA11,AD11,AG11,AJ11,AM11,AP11)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="7">
+      <c r="J11" s="7">
+        <v>14</v>
+      </c>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7">
+        <v>4</v>
+      </c>
+      <c r="N11" s="7">
+        <v>3</v>
+      </c>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="7"/>
+      <c r="Z11" s="7"/>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="7"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="7"/>
+      <c r="AF11" s="7"/>
+      <c r="AG11" s="7"/>
+      <c r="AH11" s="7"/>
+      <c r="AI11" s="7"/>
+      <c r="AJ11" s="7"/>
+      <c r="AK11" s="7"/>
+      <c r="AL11" s="7"/>
+      <c r="AM11" s="7"/>
+      <c r="AN11" s="7"/>
+      <c r="AO11" s="7"/>
+      <c r="AP11" s="7"/>
+      <c r="AQ11" s="7">
+        <f>SUM(J11,M11,P11,S11,V11,Y11,AB11,AE11,AH11,AK11,AN11)</f>
+        <v>18</v>
+      </c>
+      <c r="AR11" s="7">
+        <f>SUM(K11,N11,Q11,T11,W11,Z11,AC11,AF11,AI11,AL11,AO11)</f>
+        <v>3</v>
+      </c>
+      <c r="AS11" s="7">
+        <f>SUM(L11,O11,R11,U11,X11,AA11,AD11,AG11,AJ11,AM11,AP11)</f>
         <v>0</v>
       </c>
-      <c r="I11" s="7">
-        <v>0</v>
-      </c>
-      <c r="J11" s="7">
-        <v>1</v>
-      </c>
-      <c r="K11" s="7">
-        <v>0</v>
-      </c>
-      <c r="L11" s="7">
-        <v>0</v>
-      </c>
-      <c r="M11" s="7">
-        <v>0</v>
-      </c>
-      <c r="N11" s="7">
-        <v>0</v>
-      </c>
-      <c r="O11" s="7">
-        <v>0</v>
-      </c>
-      <c r="P11" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="7">
-        <v>0</v>
-      </c>
-      <c r="R11" s="7">
-        <v>0</v>
-      </c>
-      <c r="S11" s="7">
-        <v>0</v>
-      </c>
-      <c r="T11" s="7">
-        <v>0</v>
-      </c>
-      <c r="U11" s="7">
-        <v>0</v>
-      </c>
-      <c r="V11" s="7">
-        <v>0</v>
-      </c>
-      <c r="W11" s="7">
-        <v>0</v>
-      </c>
-      <c r="X11" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AE11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AH11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AI11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AJ11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AK11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AL11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AM11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AN11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AO11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AP11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AQ11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AR11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AS11" s="7">
-        <v>0</v>
-      </c>
-      <c r="AT11" s="7">
-        <f>SUM(J11:AS11)</f>
-        <v>1</v>
-      </c>
-      <c r="AU11" s="7">
-        <f>SUM(J11:AS11)</f>
-        <v>1</v>
-      </c>
-      <c r="AV11" s="7">
-        <f>SUM(J11:AS11)</f>
-        <v>1</v>
-      </c>
-      <c r="AW11" s="7"/>
-    </row>
-    <row r="12" spans="1:49">
+      <c r="AT11" s="7"/>
+    </row>
+    <row r="12" spans="1:46">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1314,11 +1157,8 @@
       <c r="AR12" s="4"/>
       <c r="AS12" s="4"/>
       <c r="AT12" s="4"/>
-      <c r="AU12" s="4"/>
-      <c r="AV12" s="4"/>
-      <c r="AW12" s="4"/>
-    </row>
-    <row r="13" spans="1:49">
+    </row>
+    <row r="13" spans="1:46">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1365,11 +1205,8 @@
       <c r="AR13" s="4"/>
       <c r="AS13" s="4"/>
       <c r="AT13" s="4"/>
-      <c r="AU13" s="4"/>
-      <c r="AV13" s="4"/>
-      <c r="AW13" s="4"/>
-    </row>
-    <row r="14" spans="1:49">
+    </row>
+    <row r="14" spans="1:46">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1416,11 +1253,8 @@
       <c r="AR14" s="4"/>
       <c r="AS14" s="4"/>
       <c r="AT14" s="4"/>
-      <c r="AU14" s="4"/>
-      <c r="AV14" s="4"/>
-      <c r="AW14" s="4"/>
-    </row>
-    <row r="15" spans="1:49">
+    </row>
+    <row r="15" spans="1:46">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1467,11 +1301,8 @@
       <c r="AR15" s="4"/>
       <c r="AS15" s="4"/>
       <c r="AT15" s="4"/>
-      <c r="AU15" s="4"/>
-      <c r="AV15" s="4"/>
-      <c r="AW15" s="4"/>
-    </row>
-    <row r="16" spans="1:49">
+    </row>
+    <row r="16" spans="1:46">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1518,11 +1349,8 @@
       <c r="AR16" s="4"/>
       <c r="AS16" s="4"/>
       <c r="AT16" s="4"/>
-      <c r="AU16" s="4"/>
-      <c r="AV16" s="4"/>
-      <c r="AW16" s="4"/>
-    </row>
-    <row r="17" spans="1:49">
+    </row>
+    <row r="17" spans="1:46">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1569,11 +1397,8 @@
       <c r="AR17" s="4"/>
       <c r="AS17" s="4"/>
       <c r="AT17" s="4"/>
-      <c r="AU17" s="4"/>
-      <c r="AV17" s="4"/>
-      <c r="AW17" s="4"/>
-    </row>
-    <row r="18" spans="1:49">
+    </row>
+    <row r="18" spans="1:46">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1620,11 +1445,8 @@
       <c r="AR18" s="4"/>
       <c r="AS18" s="4"/>
       <c r="AT18" s="4"/>
-      <c r="AU18" s="4"/>
-      <c r="AV18" s="4"/>
-      <c r="AW18" s="4"/>
-    </row>
-    <row r="19" spans="1:49">
+    </row>
+    <row r="19" spans="1:46">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1671,11 +1493,8 @@
       <c r="AR19" s="4"/>
       <c r="AS19" s="4"/>
       <c r="AT19" s="4"/>
-      <c r="AU19" s="4"/>
-      <c r="AV19" s="4"/>
-      <c r="AW19" s="4"/>
-    </row>
-    <row r="20" spans="1:49">
+    </row>
+    <row r="20" spans="1:46">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1722,11 +1541,8 @@
       <c r="AR20" s="4"/>
       <c r="AS20" s="4"/>
       <c r="AT20" s="4"/>
-      <c r="AU20" s="4"/>
-      <c r="AV20" s="4"/>
-      <c r="AW20" s="4"/>
-    </row>
-    <row r="21" spans="1:49">
+    </row>
+    <row r="21" spans="1:46">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1773,11 +1589,8 @@
       <c r="AR21" s="4"/>
       <c r="AS21" s="4"/>
       <c r="AT21" s="4"/>
-      <c r="AU21" s="4"/>
-      <c r="AV21" s="4"/>
-      <c r="AW21" s="4"/>
-    </row>
-    <row r="22" spans="1:49">
+    </row>
+    <row r="22" spans="1:46">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1824,11 +1637,8 @@
       <c r="AR22" s="4"/>
       <c r="AS22" s="4"/>
       <c r="AT22" s="4"/>
-      <c r="AU22" s="4"/>
-      <c r="AV22" s="4"/>
-      <c r="AW22" s="4"/>
-    </row>
-    <row r="23" spans="1:49">
+    </row>
+    <row r="23" spans="1:46">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1875,11 +1685,8 @@
       <c r="AR23" s="4"/>
       <c r="AS23" s="4"/>
       <c r="AT23" s="4"/>
-      <c r="AU23" s="4"/>
-      <c r="AV23" s="4"/>
-      <c r="AW23" s="4"/>
-    </row>
-    <row r="24" spans="1:49">
+    </row>
+    <row r="24" spans="1:46">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1926,11 +1733,8 @@
       <c r="AR24" s="4"/>
       <c r="AS24" s="4"/>
       <c r="AT24" s="4"/>
-      <c r="AU24" s="4"/>
-      <c r="AV24" s="4"/>
-      <c r="AW24" s="4"/>
-    </row>
-    <row r="25" spans="1:49">
+    </row>
+    <row r="25" spans="1:46">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1977,11 +1781,8 @@
       <c r="AR25" s="4"/>
       <c r="AS25" s="4"/>
       <c r="AT25" s="4"/>
-      <c r="AU25" s="4"/>
-      <c r="AV25" s="4"/>
-      <c r="AW25" s="4"/>
-    </row>
-    <row r="26" spans="1:49">
+    </row>
+    <row r="26" spans="1:46">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -2028,11 +1829,8 @@
       <c r="AR26" s="4"/>
       <c r="AS26" s="4"/>
       <c r="AT26" s="4"/>
-      <c r="AU26" s="4"/>
-      <c r="AV26" s="4"/>
-      <c r="AW26" s="4"/>
-    </row>
-    <row r="27" spans="1:49">
+    </row>
+    <row r="27" spans="1:46">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -2079,11 +1877,8 @@
       <c r="AR27" s="4"/>
       <c r="AS27" s="4"/>
       <c r="AT27" s="4"/>
-      <c r="AU27" s="4"/>
-      <c r="AV27" s="4"/>
-      <c r="AW27" s="4"/>
-    </row>
-    <row r="28" spans="1:49">
+    </row>
+    <row r="28" spans="1:46">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -2130,11 +1925,8 @@
       <c r="AR28" s="4"/>
       <c r="AS28" s="4"/>
       <c r="AT28" s="4"/>
-      <c r="AU28" s="4"/>
-      <c r="AV28" s="4"/>
-      <c r="AW28" s="4"/>
-    </row>
-    <row r="29" spans="1:49">
+    </row>
+    <row r="29" spans="1:46">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -2181,11 +1973,8 @@
       <c r="AR29" s="4"/>
       <c r="AS29" s="4"/>
       <c r="AT29" s="4"/>
-      <c r="AU29" s="4"/>
-      <c r="AV29" s="4"/>
-      <c r="AW29" s="4"/>
-    </row>
-    <row r="30" spans="1:49">
+    </row>
+    <row r="30" spans="1:46">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2232,11 +2021,8 @@
       <c r="AR30" s="4"/>
       <c r="AS30" s="4"/>
       <c r="AT30" s="4"/>
-      <c r="AU30" s="4"/>
-      <c r="AV30" s="4"/>
-      <c r="AW30" s="4"/>
-    </row>
-    <row r="31" spans="1:49">
+    </row>
+    <row r="31" spans="1:46">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2283,11 +2069,8 @@
       <c r="AR31" s="4"/>
       <c r="AS31" s="4"/>
       <c r="AT31" s="4"/>
-      <c r="AU31" s="4"/>
-      <c r="AV31" s="4"/>
-      <c r="AW31" s="4"/>
-    </row>
-    <row r="32" spans="1:49">
+    </row>
+    <row r="32" spans="1:46">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2334,11 +2117,8 @@
       <c r="AR32" s="4"/>
       <c r="AS32" s="4"/>
       <c r="AT32" s="4"/>
-      <c r="AU32" s="4"/>
-      <c r="AV32" s="4"/>
-      <c r="AW32" s="4"/>
-    </row>
-    <row r="33" spans="1:49">
+    </row>
+    <row r="33" spans="1:46">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2385,11 +2165,8 @@
       <c r="AR33" s="4"/>
       <c r="AS33" s="4"/>
       <c r="AT33" s="4"/>
-      <c r="AU33" s="4"/>
-      <c r="AV33" s="4"/>
-      <c r="AW33" s="4"/>
-    </row>
-    <row r="34" spans="1:49">
+    </row>
+    <row r="34" spans="1:46">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -2436,11 +2213,8 @@
       <c r="AR34" s="4"/>
       <c r="AS34" s="4"/>
       <c r="AT34" s="4"/>
-      <c r="AU34" s="4"/>
-      <c r="AV34" s="4"/>
-      <c r="AW34" s="4"/>
-    </row>
-    <row r="35" spans="1:49">
+    </row>
+    <row r="35" spans="1:46">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -2487,11 +2261,8 @@
       <c r="AR35" s="4"/>
       <c r="AS35" s="4"/>
       <c r="AT35" s="4"/>
-      <c r="AU35" s="4"/>
-      <c r="AV35" s="4"/>
-      <c r="AW35" s="4"/>
-    </row>
-    <row r="36" spans="1:49">
+    </row>
+    <row r="36" spans="1:46">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -2538,11 +2309,8 @@
       <c r="AR36" s="4"/>
       <c r="AS36" s="4"/>
       <c r="AT36" s="4"/>
-      <c r="AU36" s="4"/>
-      <c r="AV36" s="4"/>
-      <c r="AW36" s="4"/>
-    </row>
-    <row r="37" spans="1:49">
+    </row>
+    <row r="37" spans="1:46">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -2589,11 +2357,8 @@
       <c r="AR37" s="4"/>
       <c r="AS37" s="4"/>
       <c r="AT37" s="4"/>
-      <c r="AU37" s="4"/>
-      <c r="AV37" s="4"/>
-      <c r="AW37" s="4"/>
-    </row>
-    <row r="38" spans="1:49">
+    </row>
+    <row r="38" spans="1:46">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -2640,11 +2405,8 @@
       <c r="AR38" s="4"/>
       <c r="AS38" s="4"/>
       <c r="AT38" s="4"/>
-      <c r="AU38" s="4"/>
-      <c r="AV38" s="4"/>
-      <c r="AW38" s="4"/>
-    </row>
-    <row r="39" spans="1:49">
+    </row>
+    <row r="39" spans="1:46">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -2691,11 +2453,8 @@
       <c r="AR39" s="4"/>
       <c r="AS39" s="4"/>
       <c r="AT39" s="4"/>
-      <c r="AU39" s="4"/>
-      <c r="AV39" s="4"/>
-      <c r="AW39" s="4"/>
-    </row>
-    <row r="40" spans="1:49">
+    </row>
+    <row r="40" spans="1:46">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -2742,11 +2501,8 @@
       <c r="AR40" s="4"/>
       <c r="AS40" s="4"/>
       <c r="AT40" s="4"/>
-      <c r="AU40" s="4"/>
-      <c r="AV40" s="4"/>
-      <c r="AW40" s="4"/>
-    </row>
-    <row r="41" spans="1:49">
+    </row>
+    <row r="41" spans="1:46">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -2793,11 +2549,8 @@
       <c r="AR41" s="4"/>
       <c r="AS41" s="4"/>
       <c r="AT41" s="4"/>
-      <c r="AU41" s="4"/>
-      <c r="AV41" s="4"/>
-      <c r="AW41" s="4"/>
-    </row>
-    <row r="42" spans="1:49">
+    </row>
+    <row r="42" spans="1:46">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2844,11 +2597,8 @@
       <c r="AR42" s="4"/>
       <c r="AS42" s="4"/>
       <c r="AT42" s="4"/>
-      <c r="AU42" s="4"/>
-      <c r="AV42" s="4"/>
-      <c r="AW42" s="4"/>
-    </row>
-    <row r="43" spans="1:49">
+    </row>
+    <row r="43" spans="1:46">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -2895,20 +2645,20 @@
       <c r="AR43" s="4"/>
       <c r="AS43" s="4"/>
       <c r="AT43" s="4"/>
-      <c r="AU43" s="4"/>
-      <c r="AV43" s="4"/>
-      <c r="AW43" s="4"/>
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="A1:AW1"/>
-    <mergeCell ref="A2:AW2"/>
-    <mergeCell ref="A3:AW3"/>
+    <mergeCell ref="A1:AT1"/>
+    <mergeCell ref="A2:AT2"/>
+    <mergeCell ref="A3:AT3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:M4"/>
     <mergeCell ref="O4:S4"/>
     <mergeCell ref="U4:AA4"/>
-    <mergeCell ref="A5:AW5"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="AE4:AI4"/>
+    <mergeCell ref="AJ4:AT4"/>
+    <mergeCell ref="A5:AT5"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="C7:C9"/>
@@ -2918,10 +2668,10 @@
     <mergeCell ref="G7:G9"/>
     <mergeCell ref="H7:H9"/>
     <mergeCell ref="I7:I9"/>
-    <mergeCell ref="AT6:AV8"/>
-    <mergeCell ref="AW6:AW8"/>
+    <mergeCell ref="AQ6:AS8"/>
+    <mergeCell ref="AT6:AT8"/>
     <mergeCell ref="C6:I6"/>
-    <mergeCell ref="J6:AS6"/>
+    <mergeCell ref="J6:AP6"/>
     <mergeCell ref="J7:L8"/>
     <mergeCell ref="M7:O8"/>
     <mergeCell ref="P7:R8"/>
@@ -2933,7 +2683,6 @@
     <mergeCell ref="AH7:AJ8"/>
     <mergeCell ref="AK7:AM8"/>
     <mergeCell ref="AN7:AP8"/>
-    <mergeCell ref="AQ7:AS8"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true" horizontalCentered="true"/>
   <pageMargins left="0.472441" right="0.393701" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>